<commit_message>
some mislabelled "primary infection site"
</commit_message>
<xml_diff>
--- a/categorical_summary.xlsx
+++ b/categorical_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -431,28 +431,28 @@
         </is>
       </c>
       <c r="D2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2">
-        <v>3836</v>
+        <v>4022</v>
       </c>
       <c r="F2">
-        <v>8485</v>
+        <v>8671</v>
       </c>
       <c r="G2">
-        <v>1437</v>
+        <v>1566</v>
       </c>
       <c r="H2">
-        <v>1362</v>
+        <v>1404</v>
       </c>
       <c r="I2">
-        <v>3.685</v>
+        <v>3.69</v>
       </c>
       <c r="J2">
-        <v>2.4025</v>
+        <v>2.405</v>
       </c>
       <c r="K2">
-        <v>4.942500000000001</v>
+        <v>5.875</v>
       </c>
     </row>
     <row r="3">
@@ -467,28 +467,28 @@
         </is>
       </c>
       <c r="D3">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E3">
-        <v>9940</v>
+        <v>10423</v>
       </c>
       <c r="F3">
-        <v>21247</v>
+        <v>22803</v>
       </c>
       <c r="G3">
-        <v>3538</v>
+        <v>3661</v>
       </c>
       <c r="H3">
-        <v>2344</v>
+        <v>2531</v>
       </c>
       <c r="I3">
         <v>5.7</v>
       </c>
       <c r="J3">
-        <v>3.86</v>
+        <v>3.81</v>
       </c>
       <c r="K3">
-        <v>9.32</v>
+        <v>9.574999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -503,28 +503,28 @@
         </is>
       </c>
       <c r="D4">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4">
-        <v>11324</v>
+        <v>11492</v>
       </c>
       <c r="F4">
-        <v>24630</v>
+        <v>25037</v>
       </c>
       <c r="G4">
-        <v>2926</v>
+        <v>3006</v>
       </c>
       <c r="H4">
-        <v>2792</v>
+        <v>2873</v>
       </c>
       <c r="I4">
         <v>3.37</v>
       </c>
       <c r="J4">
-        <v>2.36</v>
+        <v>2.42</v>
       </c>
       <c r="K4">
-        <v>5.44</v>
+        <v>5.84</v>
       </c>
     </row>
     <row r="5">
@@ -539,28 +539,28 @@
         </is>
       </c>
       <c r="D5">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5">
-        <v>8044</v>
+        <v>8321</v>
       </c>
       <c r="F5">
-        <v>18662</v>
+        <v>18939</v>
       </c>
       <c r="G5">
-        <v>1748</v>
+        <v>1797</v>
       </c>
       <c r="H5">
-        <v>1818</v>
+        <v>1826</v>
       </c>
       <c r="I5">
-        <v>3.69</v>
+        <v>3.78</v>
       </c>
       <c r="J5">
-        <v>2.75</v>
+        <v>2.77</v>
       </c>
       <c r="K5">
-        <v>7.325</v>
+        <v>7.44</v>
       </c>
     </row>
     <row r="6">
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="D6">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>4102</v>
+        <v>4495</v>
       </c>
       <c r="F6">
-        <v>7642</v>
+        <v>8310</v>
       </c>
       <c r="G6">
-        <v>957</v>
+        <v>1049</v>
       </c>
       <c r="H6">
-        <v>574</v>
+        <v>660</v>
       </c>
       <c r="I6">
-        <v>5.994999999999999</v>
+        <v>5.21</v>
       </c>
       <c r="J6">
         <v>3.51</v>
       </c>
       <c r="K6">
-        <v>10.675</v>
+        <v>10.065</v>
       </c>
     </row>
     <row r="7">
@@ -678,28 +678,28 @@
         </is>
       </c>
       <c r="D9">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E9">
-        <v>47452</v>
+        <v>48755</v>
       </c>
       <c r="F9">
-        <v>108586</v>
+        <v>111634</v>
       </c>
       <c r="G9">
-        <v>16398</v>
+        <v>17042</v>
       </c>
       <c r="H9">
-        <v>22123</v>
+        <v>22826</v>
       </c>
       <c r="I9">
-        <v>3.36</v>
+        <v>3.41</v>
       </c>
       <c r="J9">
-        <v>1.8725</v>
+        <v>1.8575</v>
       </c>
       <c r="K9">
-        <v>5.58</v>
+        <v>6.03</v>
       </c>
     </row>
     <row r="10">
@@ -709,28 +709,28 @@
         </is>
       </c>
       <c r="D10">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10">
-        <v>4536</v>
+        <v>4878</v>
       </c>
       <c r="F10">
-        <v>9030</v>
+        <v>9611</v>
       </c>
       <c r="G10">
-        <v>2163</v>
+        <v>2232</v>
       </c>
       <c r="H10">
-        <v>963</v>
+        <v>993</v>
       </c>
       <c r="I10">
-        <v>11.535</v>
+        <v>12.6</v>
       </c>
       <c r="J10">
-        <v>4.445</v>
+        <v>4.455</v>
       </c>
       <c r="K10">
-        <v>34.9725</v>
+        <v>43.15</v>
       </c>
     </row>
     <row r="11">
@@ -1674,28 +1674,28 @@
         </is>
       </c>
       <c r="D40">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E40">
-        <v>75911</v>
+        <v>77678</v>
       </c>
       <c r="F40">
-        <v>208677</v>
+        <v>213465</v>
       </c>
       <c r="G40">
-        <v>17009.5</v>
+        <v>17497.5</v>
       </c>
       <c r="H40">
-        <v>58762.2</v>
+        <v>59716.2</v>
       </c>
       <c r="I40">
-        <v>2.62</v>
+        <v>2.72</v>
       </c>
       <c r="J40">
-        <v>0.54</v>
+        <v>0.585</v>
       </c>
       <c r="K40">
-        <v>4.59</v>
+        <v>4.73</v>
       </c>
     </row>
     <row r="41">
@@ -1897,284 +1897,253 @@
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>Primary/specific infection site</t>
+          <t>Mixed/unspecified site</t>
         </is>
       </c>
       <c r="D47">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E47">
-        <v>5381</v>
+        <v>8669</v>
       </c>
       <c r="F47">
-        <v>13851</v>
+        <v>91295</v>
       </c>
       <c r="G47">
-        <v>1810</v>
+        <v>2157</v>
       </c>
       <c r="H47">
-        <v>2129</v>
+        <v>24682</v>
       </c>
       <c r="I47">
-        <v>5.27</v>
+        <v>1.265</v>
       </c>
       <c r="J47">
-        <v>2.9525</v>
+        <v>0.46</v>
       </c>
       <c r="K47">
-        <v>10.0975</v>
+        <v>2.4375</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>Mixed/unspecified site</t>
+          <t>Intra-abdominal/hepatobiliary</t>
         </is>
       </c>
       <c r="D48">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E48">
-        <v>8669</v>
+        <v>4389</v>
       </c>
       <c r="F48">
-        <v>91295</v>
+        <v>33837</v>
       </c>
       <c r="G48">
-        <v>2157</v>
+        <v>1307</v>
       </c>
       <c r="H48">
-        <v>24682</v>
+        <v>6717</v>
       </c>
       <c r="I48">
-        <v>1.265</v>
+        <v>1.75</v>
       </c>
       <c r="J48">
-        <v>0.46</v>
+        <v>0.61</v>
       </c>
       <c r="K48">
-        <v>2.4375</v>
+        <v>2.785</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>Intra-abdominal/hepatobiliary</t>
+          <t>Urinary tract</t>
         </is>
       </c>
       <c r="D49">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E49">
-        <v>4389</v>
+        <v>3174</v>
       </c>
       <c r="F49">
-        <v>33837</v>
+        <v>6563</v>
       </c>
       <c r="G49">
-        <v>1307</v>
+        <v>567</v>
       </c>
       <c r="H49">
-        <v>6717</v>
+        <v>1150</v>
       </c>
       <c r="I49">
-        <v>1.75</v>
+        <v>1.215</v>
       </c>
       <c r="J49">
-        <v>0.61</v>
+        <v>0.3025</v>
       </c>
       <c r="K49">
-        <v>2.785</v>
+        <v>2.4275</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>Urinary tract</t>
+          <t>Skin/soft tissue</t>
         </is>
       </c>
       <c r="D50">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E50">
-        <v>3360</v>
+        <v>45956</v>
       </c>
       <c r="F50">
-        <v>6749</v>
+        <v>50271</v>
       </c>
       <c r="G50">
-        <v>593</v>
+        <v>8777</v>
       </c>
       <c r="H50">
-        <v>1176</v>
+        <v>8103</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>2.005</v>
       </c>
       <c r="J50">
-        <v>0.34</v>
+        <v>1.615</v>
       </c>
       <c r="K50">
-        <v>2.38</v>
+        <v>2.5575</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>Skin/soft tissue</t>
+          <t>Bone/joint</t>
         </is>
       </c>
       <c r="D51">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E51">
-        <v>45956</v>
+        <v>1309</v>
       </c>
       <c r="F51">
-        <v>50271</v>
+        <v>1714</v>
       </c>
       <c r="G51">
-        <v>8777</v>
+        <v>197</v>
       </c>
       <c r="H51">
-        <v>8103</v>
+        <v>289</v>
       </c>
       <c r="I51">
-        <v>2.005</v>
+        <v>2.36</v>
       </c>
       <c r="J51">
-        <v>1.615</v>
+        <v>0.91</v>
       </c>
       <c r="K51">
-        <v>2.5575</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>Bone/joint</t>
+          <t>Endocarditis</t>
         </is>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52">
-        <v>1309</v>
+        <v>44970</v>
       </c>
       <c r="F52">
-        <v>1714</v>
+        <v>48038</v>
       </c>
       <c r="G52">
-        <v>197</v>
+        <v>4503</v>
       </c>
       <c r="H52">
-        <v>289</v>
+        <v>6584</v>
       </c>
       <c r="I52">
-        <v>2.36</v>
+        <v>0.7</v>
       </c>
       <c r="J52">
-        <v>0.91</v>
+        <v>0.58</v>
       </c>
       <c r="K52">
-        <v>2.98</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>Endocarditis</t>
+          <t>Mucosal barrier injury</t>
         </is>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>44970</v>
+        <v>77</v>
       </c>
       <c r="F53">
-        <v>48038</v>
+        <v>167</v>
       </c>
       <c r="G53">
-        <v>4503</v>
+        <v>42</v>
       </c>
       <c r="H53">
-        <v>6584</v>
+        <v>52</v>
       </c>
       <c r="I53">
-        <v>0.7</v>
+        <v>2.65</v>
       </c>
       <c r="J53">
-        <v>0.58</v>
+        <v>2.65</v>
       </c>
       <c r="K53">
-        <v>1.79</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Prior colonization or infection</t>
+        </is>
+      </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Mucosal barrier injury</t>
+          <t>Prior colonization or infection</t>
         </is>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E54">
-        <v>77</v>
+        <v>5880</v>
       </c>
       <c r="F54">
-        <v>167</v>
+        <v>38251</v>
       </c>
       <c r="G54">
-        <v>42</v>
+        <v>1276</v>
       </c>
       <c r="H54">
-        <v>52</v>
+        <v>3019</v>
       </c>
       <c r="I54">
-        <v>2.65</v>
+        <v>4.365</v>
       </c>
       <c r="J54">
-        <v>2.65</v>
+        <v>2.595</v>
       </c>
       <c r="K54">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Prior colonization or infection</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Prior colonization or infection</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>28</v>
-      </c>
-      <c r="E55">
-        <v>5880</v>
-      </c>
-      <c r="F55">
-        <v>38251</v>
-      </c>
-      <c r="G55">
-        <v>1276</v>
-      </c>
-      <c r="H55">
-        <v>3019</v>
-      </c>
-      <c r="I55">
-        <v>4.365</v>
-      </c>
-      <c r="J55">
-        <v>2.595</v>
-      </c>
-      <c r="K55">
         <v>10.63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-run whole after changes to make sure code works. Only hiccup is the export to docx - not sure why, probably only for me version needs update or something
</commit_message>
<xml_diff>
--- a/categorical_summary.xlsx
+++ b/categorical_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -380,22 +380,22 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sum_resistant_tot</t>
+          <t>exposed_R</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>sum_susceptible_tot</t>
+          <t>total_R</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sum_resistant_value</t>
+          <t>exposed_S</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>sum_susceptible_value</t>
+          <t>total_S</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -417,114 +417,109 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Antibiotic exposure</t>
+          <t xml:space="preserve"> Hospital/care setting characteristics</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Beta-lactams</t>
+          <t>Admission &amp; ward characteristics</t>
         </is>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E2">
-        <v>4022</v>
+        <v>1693</v>
       </c>
       <c r="F2">
-        <v>8671</v>
+        <v>5653</v>
       </c>
       <c r="G2">
-        <v>1566</v>
+        <v>24954</v>
       </c>
       <c r="H2">
-        <v>1404</v>
+        <v>79300</v>
       </c>
       <c r="I2">
-        <v>3.69</v>
+        <v>0.72</v>
       </c>
       <c r="J2">
-        <v>2.405</v>
+        <v>0.37</v>
       </c>
       <c r="K2">
-        <v>5.875</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
+          <t>Hospital-level characteristics</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>45340</v>
+      </c>
+      <c r="F3">
+        <v>136459</v>
+      </c>
+      <c r="G3">
+        <v>49078</v>
+      </c>
+      <c r="H3">
+        <v>148347</v>
+      </c>
+      <c r="I3">
+        <v>1.06</v>
+      </c>
+      <c r="J3">
+        <v>0.62</v>
+      </c>
+      <c r="K3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Antibiotic exposure</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Prior antibiotic exposure, specific choice</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Carbapenems</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>60</v>
-      </c>
-      <c r="E3">
-        <v>10423</v>
-      </c>
-      <c r="F3">
-        <v>22803</v>
-      </c>
-      <c r="G3">
-        <v>3661</v>
-      </c>
-      <c r="H3">
-        <v>2531</v>
-      </c>
-      <c r="I3">
-        <v>5.7</v>
-      </c>
-      <c r="J3">
-        <v>3.81</v>
-      </c>
-      <c r="K3">
-        <v>9.574999999999999</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cephems</t>
+          <t>Beta-lactams</t>
         </is>
       </c>
       <c r="D4">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E4">
-        <v>11492</v>
+        <v>1331</v>
       </c>
       <c r="F4">
-        <v>25037</v>
+        <v>3887</v>
       </c>
       <c r="G4">
-        <v>3006</v>
+        <v>1165</v>
       </c>
       <c r="H4">
-        <v>2873</v>
+        <v>9312</v>
       </c>
       <c r="I4">
-        <v>3.37</v>
+        <v>4.15</v>
       </c>
       <c r="J4">
-        <v>2.42</v>
+        <v>2.41</v>
       </c>
       <c r="K4">
-        <v>5.84</v>
+        <v>5.86</v>
       </c>
     </row>
     <row r="5">
@@ -535,32 +530,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fluoroquinolones</t>
+          <t>Carbapenems</t>
         </is>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E5">
-        <v>8321</v>
+        <v>2078</v>
       </c>
       <c r="F5">
-        <v>18939</v>
+        <v>5041</v>
       </c>
       <c r="G5">
-        <v>1797</v>
+        <v>1368</v>
       </c>
       <c r="H5">
-        <v>1826</v>
+        <v>10834</v>
       </c>
       <c r="I5">
-        <v>3.78</v>
+        <v>5.71</v>
       </c>
       <c r="J5">
-        <v>2.77</v>
+        <v>4.01</v>
       </c>
       <c r="K5">
-        <v>7.44</v>
+        <v>9.550000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -571,32 +566,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Glycopeptides/oxazolidinones</t>
+          <t>Cephems</t>
         </is>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E6">
-        <v>4495</v>
+        <v>2094</v>
       </c>
       <c r="F6">
-        <v>8310</v>
+        <v>6555</v>
       </c>
       <c r="G6">
-        <v>1049</v>
+        <v>1912</v>
       </c>
       <c r="H6">
-        <v>660</v>
+        <v>16656</v>
       </c>
       <c r="I6">
-        <v>5.21</v>
+        <v>3.47</v>
       </c>
       <c r="J6">
-        <v>3.51</v>
+        <v>2.76</v>
       </c>
       <c r="K6">
-        <v>10.065</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -607,32 +602,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Other classes</t>
+          <t>Fluoroquinolones</t>
         </is>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E7">
-        <v>883</v>
+        <v>1084</v>
       </c>
       <c r="F7">
-        <v>1156</v>
+        <v>4535</v>
       </c>
       <c r="G7">
-        <v>257</v>
+        <v>1099</v>
       </c>
       <c r="H7">
-        <v>163</v>
+        <v>9809</v>
       </c>
       <c r="I7">
-        <v>3.715</v>
+        <v>3.59</v>
       </c>
       <c r="J7">
-        <v>1.9025</v>
+        <v>2.79</v>
       </c>
       <c r="K7">
-        <v>8.19</v>
+        <v>6.17</v>
       </c>
     </row>
     <row r="8">
@@ -643,187 +638,197 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tigecycline</t>
+          <t>Glycopeptides/oxazolidinones</t>
         </is>
       </c>
       <c r="D8">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E8">
-        <v>2353</v>
+        <v>886</v>
       </c>
       <c r="F8">
-        <v>5684</v>
+        <v>3740</v>
       </c>
       <c r="G8">
-        <v>379</v>
+        <v>515</v>
       </c>
       <c r="H8">
-        <v>151</v>
+        <v>6860</v>
       </c>
       <c r="I8">
-        <v>6.75</v>
+        <v>4.6</v>
       </c>
       <c r="J8">
-        <v>4.15</v>
+        <v>3.48</v>
       </c>
       <c r="K8">
-        <v>9.625</v>
+        <v>8.460000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Prior antibiotic exposure, non specific</t>
+          <t>Prior antibiotic exposure, specific choice</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Other classes</t>
         </is>
       </c>
       <c r="D9">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="E9">
-        <v>48755</v>
+        <v>3814</v>
       </c>
       <c r="F9">
-        <v>111634</v>
+        <v>10319</v>
       </c>
       <c r="G9">
-        <v>17042</v>
+        <v>3167</v>
       </c>
       <c r="H9">
-        <v>22826</v>
+        <v>22003</v>
       </c>
       <c r="I9">
-        <v>3.41</v>
+        <v>3.73</v>
       </c>
       <c r="J9">
-        <v>1.8575</v>
+        <v>2.78</v>
       </c>
       <c r="K9">
-        <v>6.03</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>Inappropriate empirical antibiotic treatment</t>
+          <t>Prior antibiotic exposure, specific choice</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Tigecycline</t>
         </is>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>4878</v>
+        <v>317</v>
       </c>
       <c r="F10">
-        <v>9611</v>
+        <v>1979</v>
       </c>
       <c r="G10">
-        <v>2232</v>
+        <v>128</v>
       </c>
       <c r="H10">
-        <v>993</v>
+        <v>5142</v>
       </c>
       <c r="I10">
-        <v>12.6</v>
+        <v>7.46</v>
       </c>
       <c r="J10">
-        <v>4.455</v>
+        <v>4.35</v>
       </c>
       <c r="K10">
-        <v>43.15</v>
+        <v>10.38</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Prior corticosteroid use</t>
+          <t>Prior antibiotic exposure, non specific</t>
         </is>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="E11">
-        <v>2078</v>
+        <v>10830</v>
       </c>
       <c r="F11">
-        <v>5625</v>
+        <v>39081</v>
       </c>
       <c r="G11">
-        <v>754</v>
+        <v>11194</v>
       </c>
       <c r="H11">
-        <v>1201</v>
+        <v>92823</v>
       </c>
       <c r="I11">
-        <v>2.195</v>
+        <v>4.17</v>
       </c>
       <c r="J11">
-        <v>1.6925</v>
+        <v>2.88</v>
       </c>
       <c r="K11">
-        <v>3.62</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Appropriate empirical antibiotic choice</t>
+          <t>In-hospital antibiotic exposure, non specific</t>
         </is>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E12">
-        <v>2146</v>
+        <v>2867</v>
       </c>
       <c r="F12">
-        <v>3038</v>
+        <v>4941</v>
       </c>
       <c r="G12">
-        <v>1160</v>
+        <v>6931</v>
       </c>
       <c r="H12">
-        <v>2433</v>
+        <v>12180</v>
       </c>
       <c r="I12">
-        <v>0.1</v>
+        <v>0.36</v>
       </c>
       <c r="J12">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="K12">
-        <v>0.43</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Prior antibiotic exposure, duration</t>
+          <t>In-hospital antibiotic exposure, specific</t>
         </is>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>277</v>
+        <v>2117</v>
       </c>
       <c r="F13">
-        <v>400</v>
+        <v>6802</v>
       </c>
       <c r="G13">
-        <v>123</v>
+        <v>1734</v>
       </c>
       <c r="H13">
-        <v>131</v>
+        <v>9650</v>
       </c>
       <c r="I13">
-        <v>1.64</v>
+        <v>4.46</v>
       </c>
       <c r="J13">
-        <v>1.64</v>
+        <v>2.33</v>
       </c>
       <c r="K13">
-        <v>1.64</v>
+        <v>10.21</v>
       </c>
     </row>
     <row r="14">
@@ -834,1317 +839,2164 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Low blood values</t>
+          <t>Hematology markers</t>
         </is>
       </c>
       <c r="D14">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14">
-        <v>3223</v>
+        <v>1212</v>
       </c>
       <c r="F14">
-        <v>8971</v>
+        <v>2653</v>
       </c>
       <c r="G14">
-        <v>1648</v>
+        <v>2139</v>
       </c>
       <c r="H14">
-        <v>4651</v>
+        <v>6215</v>
       </c>
       <c r="I14">
-        <v>2.97</v>
+        <v>2.94</v>
       </c>
       <c r="J14">
-        <v>1.86</v>
+        <v>1.82</v>
       </c>
       <c r="K14">
-        <v>5.32</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Clinical presentation</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Clinical severity</t>
+          <t>Liver markers</t>
         </is>
       </c>
       <c r="D15">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>6634</v>
+        <v>299</v>
       </c>
       <c r="F15">
-        <v>11921</v>
+        <v>961</v>
       </c>
       <c r="G15">
-        <v>2745</v>
+        <v>2695</v>
       </c>
       <c r="H15">
-        <v>2521</v>
+        <v>2941</v>
       </c>
       <c r="I15">
-        <v>2.98</v>
+        <v>3.37</v>
       </c>
       <c r="J15">
-        <v>1.65</v>
+        <v>3.35</v>
       </c>
       <c r="K15">
-        <v>5.3425</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>Clinical presentation, other than infection site</t>
+          <t>Metabolic markers</t>
         </is>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>1282</v>
+        <v>42</v>
       </c>
       <c r="F16">
-        <v>2833</v>
+        <v>141</v>
       </c>
       <c r="G16">
-        <v>666</v>
+        <v>133</v>
       </c>
       <c r="H16">
-        <v>1222</v>
+        <v>508</v>
       </c>
       <c r="I16">
-        <v>2.45</v>
+        <v>1.32</v>
       </c>
       <c r="J16">
-        <v>1.15</v>
+        <v>0.88</v>
       </c>
       <c r="K16">
-        <v>3.725</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Clinical presentation</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Preterm birth/low birth weight</t>
+          <t>Clinical severity, infection site</t>
         </is>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E17">
-        <v>1041</v>
+        <v>1461</v>
       </c>
       <c r="F17">
-        <v>1394</v>
+        <v>4085</v>
       </c>
       <c r="G17">
-        <v>326</v>
+        <v>1744</v>
       </c>
       <c r="H17">
-        <v>427</v>
+        <v>8701</v>
       </c>
       <c r="I17">
-        <v>3.575</v>
+        <v>3.06</v>
       </c>
       <c r="J17">
-        <v>1.1</v>
+        <v>2</v>
       </c>
       <c r="K17">
-        <v>5.475</v>
+        <v>5.35</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Comorbidities</t>
-        </is>
-      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Comorbidities</t>
+          <t>Clinical severity score</t>
         </is>
       </c>
       <c r="D18">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <v>227947</v>
+        <v>793</v>
       </c>
       <c r="F18">
-        <v>550426</v>
+        <v>2165</v>
       </c>
       <c r="G18">
-        <v>42798</v>
+        <v>1084</v>
       </c>
       <c r="H18">
-        <v>68278</v>
+        <v>3700</v>
       </c>
       <c r="I18">
-        <v>2.08</v>
+        <v>2.18</v>
       </c>
       <c r="J18">
-        <v>0.79</v>
+        <v>0.75</v>
       </c>
       <c r="K18">
-        <v>3.63</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>NCDs</t>
+          <t>Clinical presentation, other than infection site</t>
         </is>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>6310</v>
+        <v>783</v>
       </c>
       <c r="F19">
-        <v>38850</v>
+        <v>961</v>
       </c>
       <c r="G19">
-        <v>1928</v>
+        <v>1334</v>
       </c>
       <c r="H19">
-        <v>9341</v>
+        <v>2164</v>
       </c>
       <c r="I19">
-        <v>2.32</v>
+        <v>1.74</v>
       </c>
       <c r="J19">
-        <v>1.535</v>
+        <v>0.57</v>
       </c>
       <c r="K19">
-        <v>3.59</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Comorbidities</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Comorbidity score, high (Charlson &gt;2;Elixhauser&gt;13)</t>
+          <t>Cancer/hematologic malignancy</t>
         </is>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E20">
-        <v>272</v>
+        <v>8904</v>
       </c>
       <c r="F20">
-        <v>1277</v>
+        <v>57581</v>
       </c>
       <c r="G20">
-        <v>71</v>
+        <v>12975</v>
       </c>
       <c r="H20">
-        <v>439</v>
+        <v>75990</v>
       </c>
       <c r="I20">
-        <v>1.76</v>
+        <v>1.11</v>
       </c>
       <c r="J20">
-        <v>1.38</v>
+        <v>0.41</v>
       </c>
       <c r="K20">
-        <v>2.14</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Demographics</t>
-        </is>
-      </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Male sex</t>
+          <t>Immunosuppression/ immunocompromised state</t>
         </is>
       </c>
       <c r="D21">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21">
-        <v>64512</v>
+        <v>2654</v>
       </c>
       <c r="F21">
-        <v>231896</v>
+        <v>51658</v>
       </c>
       <c r="G21">
-        <v>37630</v>
+        <v>3043</v>
       </c>
       <c r="H21">
-        <v>111222</v>
+        <v>58908</v>
       </c>
       <c r="I21">
-        <v>1.705</v>
+        <v>2.13</v>
       </c>
       <c r="J21">
-        <v>1.355</v>
+        <v>0.95</v>
       </c>
       <c r="K21">
-        <v>2.44</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>Older age (cutoffs &gt;/= 60 years)</t>
+          <t>Kidney/ renal disease</t>
         </is>
       </c>
       <c r="D22">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E22">
-        <v>47747</v>
+        <v>2308</v>
       </c>
       <c r="F22">
-        <v>53132</v>
+        <v>6545</v>
       </c>
       <c r="G22">
-        <v>9881</v>
+        <v>6515</v>
       </c>
       <c r="H22">
-        <v>9751</v>
+        <v>36859</v>
       </c>
       <c r="I22">
-        <v>1.54</v>
+        <v>2.88</v>
       </c>
       <c r="J22">
-        <v>0.7625</v>
+        <v>1.98</v>
       </c>
       <c r="K22">
-        <v>1.805</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>Young age (cutoffs &lt;/= 5 years)</t>
+          <t>Cardiovascular &amp; cerebrovascular disease</t>
         </is>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E23">
-        <v>2157</v>
+        <v>14543</v>
       </c>
       <c r="F23">
-        <v>4322</v>
+        <v>54298</v>
       </c>
       <c r="G23">
-        <v>156</v>
+        <v>22284</v>
       </c>
       <c r="H23">
-        <v>519</v>
+        <v>163644</v>
       </c>
       <c r="I23">
-        <v>0.95</v>
+        <v>3.05</v>
       </c>
       <c r="J23">
-        <v>0.51</v>
+        <v>1.75</v>
       </c>
       <c r="K23">
-        <v>0.95</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>Geography</t>
+          <t>Liver/ Gastrointestinal/ biliary disease</t>
         </is>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E24">
-        <v>323791</v>
+        <v>885</v>
       </c>
       <c r="F24">
-        <v>423356</v>
+        <v>6567</v>
       </c>
       <c r="G24">
-        <v>93284</v>
+        <v>3153</v>
       </c>
       <c r="H24">
-        <v>124824</v>
+        <v>60802</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>2.14</v>
       </c>
       <c r="J24">
-        <v>0.8300000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="K24">
-        <v>1.33</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Metabolic/endocrine</t>
         </is>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E25">
-        <v>977</v>
+        <v>1639</v>
       </c>
       <c r="F25">
-        <v>4024</v>
+        <v>5419</v>
       </c>
       <c r="G25">
-        <v>137</v>
+        <v>8908</v>
       </c>
       <c r="H25">
-        <v>538</v>
+        <v>36738</v>
       </c>
       <c r="I25">
-        <v>4.955</v>
+        <v>1.92</v>
       </c>
       <c r="J25">
-        <v>2.5275</v>
+        <v>1.4</v>
       </c>
       <c r="K25">
-        <v>6.0175</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Healthcare exposure</t>
-        </is>
-      </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Prior hospitalisation</t>
+          <t>Respiratory disease</t>
         </is>
       </c>
       <c r="D26">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="E26">
-        <v>204212</v>
+        <v>13341</v>
       </c>
       <c r="F26">
-        <v>288911</v>
+        <v>48581</v>
       </c>
       <c r="G26">
-        <v>62195</v>
+        <v>14610</v>
       </c>
       <c r="H26">
-        <v>69617</v>
+        <v>80346</v>
       </c>
       <c r="I26">
-        <v>2.74</v>
+        <v>3.73</v>
       </c>
       <c r="J26">
-        <v>1.49</v>
+        <v>2.59</v>
       </c>
       <c r="K26">
-        <v>4.045</v>
+        <v>4.78</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>Prior ICU stay</t>
+          <t>Neurologic/ cognitive/ functional status</t>
         </is>
       </c>
       <c r="D27">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="E27">
-        <v>13896</v>
+        <v>731</v>
       </c>
       <c r="F27">
-        <v>56231</v>
+        <v>3011</v>
       </c>
       <c r="G27">
-        <v>6459</v>
+        <v>2372</v>
       </c>
       <c r="H27">
-        <v>16457</v>
+        <v>29792</v>
       </c>
       <c r="I27">
-        <v>3.16</v>
+        <v>2.94</v>
       </c>
       <c r="J27">
-        <v>1.835</v>
+        <v>2.19</v>
       </c>
       <c r="K27">
-        <v>7.87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>Hospital-acquired</t>
+          <t>Other chronic condition</t>
         </is>
       </c>
       <c r="D28">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E28">
-        <v>8661</v>
+        <v>208</v>
       </c>
       <c r="F28">
-        <v>42568</v>
+        <v>973</v>
       </c>
       <c r="G28">
-        <v>4928</v>
+        <v>366</v>
       </c>
       <c r="H28">
-        <v>10296</v>
+        <v>2962</v>
       </c>
       <c r="I28">
-        <v>3</v>
+        <v>2.82</v>
       </c>
       <c r="J28">
-        <v>2.01</v>
+        <v>2.18</v>
       </c>
       <c r="K28">
-        <v>7.39</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>Community-acquired</t>
+          <t>Autoimmune/ rheumatologic/ collective tissue disease</t>
         </is>
       </c>
       <c r="D29">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>17240</v>
+        <v>100</v>
       </c>
       <c r="F29">
-        <v>59513</v>
+        <v>1614</v>
       </c>
       <c r="G29">
-        <v>4627</v>
+        <v>667</v>
       </c>
       <c r="H29">
-        <v>26575</v>
+        <v>28740</v>
       </c>
       <c r="I29">
-        <v>0.35</v>
+        <v>0.98</v>
       </c>
       <c r="J29">
-        <v>0.2225</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>0.6</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>Healthcare associated, other than hospital-acquired or non specified if hospital</t>
+          <t>Comorbidity score</t>
         </is>
       </c>
       <c r="D30">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>4601</v>
+        <v>1034</v>
       </c>
       <c r="F30">
-        <v>35150</v>
+        <v>2627</v>
       </c>
       <c r="G30">
-        <v>2765</v>
+        <v>7332</v>
       </c>
       <c r="H30">
-        <v>10714</v>
+        <v>30474</v>
       </c>
       <c r="I30">
-        <v>2.93</v>
+        <v>1.32</v>
       </c>
       <c r="J30">
-        <v>2.16</v>
+        <v>0.72</v>
       </c>
       <c r="K30">
-        <v>6.59</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>Long-term care facility</t>
+          <t>Urologic disease</t>
         </is>
       </c>
       <c r="D31">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <v>2688</v>
+        <v>225</v>
       </c>
       <c r="F31">
-        <v>5963</v>
+        <v>885</v>
       </c>
       <c r="G31">
-        <v>749</v>
+        <v>156</v>
       </c>
       <c r="H31">
-        <v>631</v>
+        <v>1014</v>
       </c>
       <c r="I31">
-        <v>4.84</v>
+        <v>2.54</v>
       </c>
       <c r="J31">
-        <v>4.295</v>
+        <v>2.33</v>
       </c>
       <c r="K31">
-        <v>6.257499999999999</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Invasive procedures</t>
-        </is>
-      </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gastrointestinal/urinary tubes or drains</t>
+          <t>Underweight/malnutrition</t>
         </is>
       </c>
       <c r="D32">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>17242</v>
+        <v>384</v>
       </c>
       <c r="F32">
-        <v>39802</v>
+        <v>762</v>
       </c>
       <c r="G32">
-        <v>7587</v>
+        <v>56</v>
       </c>
       <c r="H32">
-        <v>9319</v>
+        <v>168</v>
       </c>
       <c r="I32">
-        <v>3.37</v>
+        <v>1.96</v>
       </c>
       <c r="J32">
-        <v>2.19</v>
+        <v>1.91</v>
       </c>
       <c r="K32">
-        <v>5.6</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Airway/respiratory procedures</t>
+          <t>Male sex</t>
         </is>
       </c>
       <c r="D33">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E33">
-        <v>15162</v>
+        <v>36604</v>
       </c>
       <c r="F33">
-        <v>41750</v>
+        <v>64512</v>
       </c>
       <c r="G33">
-        <v>4924</v>
+        <v>124234</v>
       </c>
       <c r="H33">
-        <v>6515</v>
+        <v>231896</v>
       </c>
       <c r="I33">
-        <v>4.21</v>
+        <v>1.63</v>
       </c>
       <c r="J33">
-        <v>2.085</v>
+        <v>0.72</v>
       </c>
       <c r="K33">
-        <v>7.347499999999999</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>Surgery / Invasive procedure</t>
+          <t>Older age (cutoffs &gt;/= 60 years)</t>
         </is>
       </c>
       <c r="D34">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>10207</v>
+        <v>9935</v>
       </c>
       <c r="F34">
-        <v>18920</v>
+        <v>47985</v>
       </c>
       <c r="G34">
-        <v>3045</v>
+        <v>10372</v>
       </c>
       <c r="H34">
-        <v>3577</v>
+        <v>54290</v>
       </c>
       <c r="I34">
-        <v>2.86</v>
+        <v>1.54</v>
       </c>
       <c r="J34">
-        <v>1.935</v>
+        <v>0.66</v>
       </c>
       <c r="K34">
-        <v>5.045</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>Central venous access/dialysis</t>
+          <t>Young age (cutoffs &lt;/= 5 years)</t>
         </is>
       </c>
       <c r="D35">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E35">
-        <v>49503</v>
+        <v>210</v>
       </c>
       <c r="F35">
-        <v>58092</v>
+        <v>3330</v>
       </c>
       <c r="G35">
-        <v>7804</v>
+        <v>557</v>
       </c>
       <c r="H35">
-        <v>9296</v>
+        <v>7501</v>
       </c>
       <c r="I35">
-        <v>4.03</v>
+        <v>0.95</v>
       </c>
       <c r="J35">
-        <v>2.26</v>
+        <v>0.73</v>
       </c>
       <c r="K35">
-        <v>6.3</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>Internal device / implant</t>
+          <t>Ethnicity</t>
         </is>
       </c>
       <c r="D36">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>9505</v>
+        <v>149</v>
       </c>
       <c r="F36">
-        <v>12956</v>
+        <v>1109</v>
       </c>
       <c r="G36">
-        <v>4219</v>
+        <v>750</v>
       </c>
       <c r="H36">
-        <v>3157</v>
+        <v>4652</v>
       </c>
       <c r="I36">
-        <v>2.97</v>
+        <v>2</v>
       </c>
       <c r="J36">
-        <v>2.34</v>
+        <v>0.34</v>
       </c>
       <c r="K36">
-        <v>7.8</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>Transplant</t>
+          <t>Socio-economic status</t>
         </is>
       </c>
       <c r="D37">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E37">
-        <v>49142</v>
+        <v>89214</v>
       </c>
       <c r="F37">
-        <v>56252</v>
+        <v>315009</v>
       </c>
       <c r="G37">
-        <v>1469</v>
+        <v>95063</v>
       </c>
       <c r="H37">
-        <v>1805</v>
+        <v>338806</v>
       </c>
       <c r="I37">
-        <v>3.88</v>
+        <v>0.88</v>
       </c>
       <c r="J37">
-        <v>1.54</v>
+        <v>0.49</v>
       </c>
       <c r="K37">
-        <v>7.76</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>Prior IV therapy</t>
+          <t>Geography</t>
         </is>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E38">
-        <v>932</v>
+        <v>4127</v>
       </c>
       <c r="F38">
-        <v>2017</v>
+        <v>10140</v>
       </c>
       <c r="G38">
-        <v>578</v>
+        <v>30127</v>
       </c>
       <c r="H38">
-        <v>556</v>
+        <v>89300</v>
       </c>
       <c r="I38">
-        <v>2.32</v>
+        <v>1</v>
       </c>
       <c r="J38">
-        <v>0.28</v>
+        <v>1</v>
       </c>
       <c r="K38">
-        <v>3.66</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Healthcare exposure</t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Blood transfusion</t>
+          <t>Hospital-acquired</t>
         </is>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="E39">
-        <v>298</v>
+        <v>8261</v>
       </c>
       <c r="F39">
-        <v>1167</v>
+        <v>13824</v>
       </c>
       <c r="G39">
-        <v>141</v>
+        <v>12674</v>
       </c>
       <c r="H39">
-        <v>350</v>
+        <v>51859</v>
       </c>
       <c r="I39">
-        <v>2.235</v>
+        <v>2.84</v>
       </c>
       <c r="J39">
-        <v>2.1075</v>
+        <v>1.52</v>
       </c>
       <c r="K39">
-        <v>2.4475</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Prior hospitalisation</t>
         </is>
       </c>
       <c r="D40">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="E40">
-        <v>77678</v>
+        <v>6440</v>
       </c>
       <c r="F40">
-        <v>213465</v>
+        <v>13518</v>
       </c>
       <c r="G40">
-        <v>17497.5</v>
+        <v>9639</v>
       </c>
       <c r="H40">
-        <v>59716.2</v>
+        <v>43933</v>
       </c>
       <c r="I40">
-        <v>2.72</v>
+        <v>2.64</v>
       </c>
       <c r="J40">
-        <v>0.585</v>
+        <v>1.61</v>
       </c>
       <c r="K40">
-        <v>4.73</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Patient outcomes</t>
-        </is>
-      </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Patient outcomes, mortality</t>
+          <t>Healthcare associated, other than hospital-acquired or non specified if hospital</t>
         </is>
       </c>
       <c r="D41">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="E41">
-        <v>17036</v>
+        <v>3142</v>
       </c>
       <c r="F41">
-        <v>41130</v>
+        <v>6073</v>
       </c>
       <c r="G41">
-        <v>5710</v>
+        <v>11085</v>
       </c>
       <c r="H41">
-        <v>5796</v>
+        <v>37692</v>
       </c>
       <c r="I41">
-        <v>3.25</v>
+        <v>2.93</v>
       </c>
       <c r="J41">
-        <v>2.155</v>
+        <v>1.88</v>
       </c>
       <c r="K41">
-        <v>6.85</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>Patient outcomes, cure</t>
+          <t>Community-acquired</t>
         </is>
       </c>
       <c r="D42">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E42">
-        <v>779</v>
+        <v>3015</v>
       </c>
       <c r="F42">
-        <v>1803</v>
+        <v>6912</v>
       </c>
       <c r="G42">
-        <v>498</v>
+        <v>24017</v>
       </c>
       <c r="H42">
-        <v>1869</v>
+        <v>38758</v>
       </c>
       <c r="I42">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
       <c r="J42">
-        <v>0.1725</v>
+        <v>0.2</v>
       </c>
       <c r="K42">
-        <v>0.425</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Patient outcomes, complications</t>
+          <t>Prior ICU stay</t>
         </is>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E43">
-        <v>435</v>
+        <v>1194</v>
       </c>
       <c r="F43">
-        <v>1280</v>
+        <v>2878</v>
       </c>
       <c r="G43">
-        <v>108</v>
+        <v>1114</v>
       </c>
       <c r="H43">
-        <v>104</v>
+        <v>6621</v>
       </c>
       <c r="I43">
-        <v>4.67</v>
+        <v>4.4</v>
       </c>
       <c r="J43">
-        <v>2.6</v>
+        <v>3.17</v>
       </c>
       <c r="K43">
-        <v>5.02</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>Patient outcomes, treatment failure</t>
+          <t>Long-term care facility</t>
         </is>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E44">
-        <v>452</v>
+        <v>888</v>
       </c>
       <c r="F44">
-        <v>1306</v>
+        <v>3747</v>
       </c>
       <c r="G44">
-        <v>295</v>
+        <v>1902</v>
       </c>
       <c r="H44">
-        <v>552</v>
+        <v>18618</v>
       </c>
       <c r="I44">
-        <v>3.2</v>
+        <v>4.53</v>
       </c>
       <c r="J44">
-        <v>2.2625</v>
+        <v>2.93</v>
       </c>
       <c r="K44">
-        <v>4.6</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Invasive procedures/devices</t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Patient outcomes, duration of hospitalisation or treatment</t>
+          <t>Central venous/intravascular access &amp; dialysis</t>
         </is>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="E45">
-        <v>350</v>
+        <v>13327</v>
       </c>
       <c r="F45">
-        <v>11519</v>
+        <v>60023</v>
       </c>
       <c r="G45">
-        <v>87</v>
+        <v>15775</v>
       </c>
       <c r="H45">
-        <v>1199</v>
+        <v>79192</v>
       </c>
       <c r="I45">
-        <v>1.87</v>
+        <v>3.18</v>
       </c>
       <c r="J45">
-        <v>1.315</v>
+        <v>2.15</v>
       </c>
       <c r="K45">
-        <v>2.425</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Primary/specific infection site</t>
-        </is>
-      </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Respiratory tract/pulmonary</t>
+          <t>Airway/respiratory procedures</t>
         </is>
       </c>
       <c r="D46">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="E46">
-        <v>49461</v>
+        <v>4570</v>
       </c>
       <c r="F46">
-        <v>60301</v>
+        <v>13134</v>
       </c>
       <c r="G46">
-        <v>15343</v>
+        <v>5490</v>
       </c>
       <c r="H46">
-        <v>13420</v>
+        <v>33227</v>
       </c>
       <c r="I46">
-        <v>3.57</v>
+        <v>4.36</v>
       </c>
       <c r="J46">
-        <v>2.3375</v>
+        <v>2.51</v>
       </c>
       <c r="K46">
-        <v>5.3</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>Mixed/unspecified site</t>
+          <t>Urinary catheters/urinary procedures</t>
         </is>
       </c>
       <c r="D47">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E47">
-        <v>8669</v>
+        <v>3158</v>
       </c>
       <c r="F47">
-        <v>91295</v>
+        <v>7212</v>
       </c>
       <c r="G47">
-        <v>2157</v>
+        <v>3678</v>
       </c>
       <c r="H47">
-        <v>24682</v>
+        <v>18670</v>
       </c>
       <c r="I47">
-        <v>1.265</v>
+        <v>3.63</v>
       </c>
       <c r="J47">
-        <v>0.46</v>
+        <v>2.47</v>
       </c>
       <c r="K47">
-        <v>2.4375</v>
+        <v>6.02</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>Intra-abdominal/hepatobiliary</t>
+          <t>Surgery/invasive operation</t>
         </is>
       </c>
       <c r="D48">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E48">
-        <v>4389</v>
+        <v>3125</v>
       </c>
       <c r="F48">
-        <v>33837</v>
+        <v>10767</v>
       </c>
       <c r="G48">
-        <v>1307</v>
+        <v>3451</v>
       </c>
       <c r="H48">
-        <v>6717</v>
+        <v>18924</v>
       </c>
       <c r="I48">
-        <v>1.75</v>
+        <v>2.81</v>
       </c>
       <c r="J48">
-        <v>0.61</v>
+        <v>1.92</v>
       </c>
       <c r="K48">
-        <v>2.785</v>
+        <v>5.52</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>Urinary tract</t>
+          <t>Gastrointestinal/biliary tubes &amp; abdominal drains</t>
         </is>
       </c>
       <c r="D49">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E49">
-        <v>3174</v>
+        <v>3463</v>
       </c>
       <c r="F49">
-        <v>6563</v>
+        <v>10287</v>
       </c>
       <c r="G49">
-        <v>567</v>
+        <v>3967</v>
       </c>
       <c r="H49">
-        <v>1150</v>
+        <v>23302</v>
       </c>
       <c r="I49">
-        <v>1.215</v>
+        <v>3.23</v>
       </c>
       <c r="J49">
-        <v>0.3025</v>
+        <v>2.13</v>
       </c>
       <c r="K49">
-        <v>2.4275</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>Skin/soft tissue</t>
+          <t>Transplant</t>
         </is>
       </c>
       <c r="D50">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E50">
-        <v>45956</v>
+        <v>1516</v>
       </c>
       <c r="F50">
-        <v>50271</v>
+        <v>49392</v>
       </c>
       <c r="G50">
-        <v>8777</v>
+        <v>1849</v>
       </c>
       <c r="H50">
-        <v>8103</v>
+        <v>56712</v>
       </c>
       <c r="I50">
-        <v>2.005</v>
+        <v>3.58</v>
       </c>
       <c r="J50">
-        <v>1.615</v>
+        <v>1.47</v>
       </c>
       <c r="K50">
-        <v>2.5575</v>
+        <v>6.21</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>Bone/joint</t>
+          <t>Invasive devices/procedures, unspecified</t>
         </is>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E51">
-        <v>1309</v>
+        <v>1209</v>
       </c>
       <c r="F51">
-        <v>1714</v>
+        <v>2067</v>
       </c>
       <c r="G51">
-        <v>197</v>
+        <v>1037</v>
       </c>
       <c r="H51">
-        <v>289</v>
+        <v>2879</v>
       </c>
       <c r="I51">
-        <v>2.36</v>
+        <v>3.16</v>
       </c>
       <c r="J51">
-        <v>0.91</v>
+        <v>2.73</v>
       </c>
       <c r="K51">
-        <v>2.98</v>
+        <v>4.96</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>Endocarditis</t>
+          <t>Blood transfusion</t>
         </is>
       </c>
       <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>253</v>
+      </c>
+      <c r="F52">
+        <v>544</v>
+      </c>
+      <c r="G52">
+        <v>417</v>
+      </c>
+      <c r="H52">
+        <v>1414</v>
+      </c>
+      <c r="I52">
+        <v>2.54</v>
+      </c>
+      <c r="J52">
+        <v>2.17</v>
+      </c>
+      <c r="K52">
         <v>3</v>
-      </c>
-      <c r="E52">
-        <v>44970</v>
-      </c>
-      <c r="F52">
-        <v>48038</v>
-      </c>
-      <c r="G52">
-        <v>4503</v>
-      </c>
-      <c r="H52">
-        <v>6584</v>
-      </c>
-      <c r="I52">
-        <v>0.7</v>
-      </c>
-      <c r="J52">
-        <v>0.58</v>
-      </c>
-      <c r="K52">
-        <v>1.79</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>Mucosal barrier injury</t>
+          <t>Internal device/implant</t>
         </is>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F53">
-        <v>167</v>
+        <v>387</v>
       </c>
       <c r="G53">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="H53">
-        <v>52</v>
+        <v>342</v>
       </c>
       <c r="I53">
-        <v>2.65</v>
+        <v>1.7</v>
       </c>
       <c r="J53">
-        <v>2.65</v>
+        <v>0.92</v>
       </c>
       <c r="K53">
-        <v>2.65</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>Neonatal risk</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Birthweight</t>
+        </is>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>95</v>
+      </c>
+      <c r="F54">
+        <v>311</v>
+      </c>
+      <c r="G54">
+        <v>188</v>
+      </c>
+      <c r="H54">
+        <v>501</v>
+      </c>
+      <c r="I54">
+        <v>2.98</v>
+      </c>
+      <c r="J54">
+        <v>0.7</v>
+      </c>
+      <c r="K54">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Gestational age</t>
+        </is>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>298</v>
+      </c>
+      <c r="F55">
+        <v>818</v>
+      </c>
+      <c r="G55">
+        <v>287</v>
+      </c>
+      <c r="H55">
+        <v>1029</v>
+      </c>
+      <c r="I55">
+        <v>5.4</v>
+      </c>
+      <c r="J55">
+        <v>1.92</v>
+      </c>
+      <c r="K55">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Feeding type</t>
+        </is>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>29</v>
+      </c>
+      <c r="F56">
+        <v>116</v>
+      </c>
+      <c r="G56">
+        <v>44</v>
+      </c>
+      <c r="H56">
+        <v>200</v>
+      </c>
+      <c r="I56">
+        <v>1.83</v>
+      </c>
+      <c r="J56">
+        <v>1.13</v>
+      </c>
+      <c r="K56">
+        <v>2.53</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D57">
+        <v>47</v>
+      </c>
+      <c r="E57">
+        <v>3511</v>
+      </c>
+      <c r="F57">
+        <v>10213</v>
+      </c>
+      <c r="G57">
+        <v>16737</v>
+      </c>
+      <c r="H57">
+        <v>41868</v>
+      </c>
+      <c r="I57">
+        <v>2.58</v>
+      </c>
+      <c r="J57">
+        <v>0.48</v>
+      </c>
+      <c r="K57">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Invasive devices, unspecified</t>
+        </is>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>116</v>
+      </c>
+      <c r="F58">
+        <v>210</v>
+      </c>
+      <c r="G58">
+        <v>263</v>
+      </c>
+      <c r="H58">
+        <v>678</v>
+      </c>
+      <c r="I58">
+        <v>3.75</v>
+      </c>
+      <c r="J58">
+        <v>3.34</v>
+      </c>
+      <c r="K58">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Patient outcomes</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Mortality</t>
+        </is>
+      </c>
+      <c r="D59">
+        <v>90</v>
+      </c>
+      <c r="E59">
+        <v>14268</v>
+      </c>
+      <c r="F59">
+        <v>73896</v>
+      </c>
+      <c r="G59">
+        <v>14367</v>
+      </c>
+      <c r="H59">
+        <v>115506</v>
+      </c>
+      <c r="I59">
+        <v>3.48</v>
+      </c>
+      <c r="J59">
+        <v>2.16</v>
+      </c>
+      <c r="K59">
+        <v>6.62</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Current ICU stay</t>
+        </is>
+      </c>
+      <c r="D60">
+        <v>41</v>
+      </c>
+      <c r="E60">
+        <v>3454</v>
+      </c>
+      <c r="F60">
+        <v>8412</v>
+      </c>
+      <c r="G60">
+        <v>14489</v>
+      </c>
+      <c r="H60">
+        <v>43978</v>
+      </c>
+      <c r="I60">
+        <v>2.59</v>
+      </c>
+      <c r="J60">
+        <v>1.81</v>
+      </c>
+      <c r="K60">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Complications</t>
+        </is>
+      </c>
+      <c r="D61">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>513</v>
+      </c>
+      <c r="F61">
+        <v>2159</v>
+      </c>
+      <c r="G61">
+        <v>509</v>
+      </c>
+      <c r="H61">
+        <v>3811</v>
+      </c>
+      <c r="I61">
+        <v>2.51</v>
+      </c>
+      <c r="J61">
+        <v>2.12</v>
+      </c>
+      <c r="K61">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Current hospitalisation duration</t>
+        </is>
+      </c>
+      <c r="D62">
+        <v>9</v>
+      </c>
+      <c r="E62">
+        <v>484</v>
+      </c>
+      <c r="F62">
+        <v>1391</v>
+      </c>
+      <c r="G62">
+        <v>2596</v>
+      </c>
+      <c r="H62">
+        <v>24145</v>
+      </c>
+      <c r="I62">
+        <v>2.75</v>
+      </c>
+      <c r="J62">
+        <v>1.38</v>
+      </c>
+      <c r="K62">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Cure</t>
+        </is>
+      </c>
+      <c r="D63">
+        <v>8</v>
+      </c>
+      <c r="E63">
+        <v>648</v>
+      </c>
+      <c r="F63">
+        <v>975</v>
+      </c>
+      <c r="G63">
+        <v>2449</v>
+      </c>
+      <c r="H63">
+        <v>2465</v>
+      </c>
+      <c r="I63">
+        <v>0.22</v>
+      </c>
+      <c r="J63">
+        <v>0.2</v>
+      </c>
+      <c r="K63">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Treatment failure</t>
+        </is>
+      </c>
+      <c r="D64">
+        <v>8</v>
+      </c>
+      <c r="E64">
+        <v>790</v>
+      </c>
+      <c r="F64">
+        <v>1536</v>
+      </c>
+      <c r="G64">
+        <v>567</v>
+      </c>
+      <c r="H64">
+        <v>2916</v>
+      </c>
+      <c r="I64">
+        <v>4.36</v>
+      </c>
+      <c r="J64">
+        <v>2.69</v>
+      </c>
+      <c r="K64">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Persistent bacteremia</t>
+        </is>
+      </c>
+      <c r="D65">
+        <v>6</v>
+      </c>
+      <c r="E65">
+        <v>215</v>
+      </c>
+      <c r="F65">
+        <v>796</v>
+      </c>
+      <c r="G65">
+        <v>221</v>
+      </c>
+      <c r="H65">
+        <v>2339</v>
+      </c>
+      <c r="I65">
+        <v>5.42</v>
+      </c>
+      <c r="J65">
+        <v>3.44</v>
+      </c>
+      <c r="K65">
+        <v>10.41</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Readmission</t>
+        </is>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>245</v>
+      </c>
+      <c r="F66">
+        <v>1577</v>
+      </c>
+      <c r="G66">
+        <v>1951</v>
+      </c>
+      <c r="H66">
+        <v>35519</v>
+      </c>
+      <c r="I66">
+        <v>2.64</v>
+      </c>
+      <c r="J66">
+        <v>1.53</v>
+      </c>
+      <c r="K66">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Fever</t>
+        </is>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>64</v>
+      </c>
+      <c r="F67">
+        <v>92</v>
+      </c>
+      <c r="G67">
+        <v>39</v>
+      </c>
+      <c r="H67">
+        <v>147</v>
+      </c>
+      <c r="I67">
+        <v>6.33</v>
+      </c>
+      <c r="J67">
+        <v>6.33</v>
+      </c>
+      <c r="K67">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Primary site of infection</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Respiratory tract/pulmonary</t>
+        </is>
+      </c>
+      <c r="D68">
+        <v>26</v>
+      </c>
+      <c r="E68">
+        <v>14837</v>
+      </c>
+      <c r="F68">
+        <v>48102</v>
+      </c>
+      <c r="G68">
+        <v>13025</v>
+      </c>
+      <c r="H68">
+        <v>55958</v>
+      </c>
+      <c r="I68">
+        <v>3.09</v>
+      </c>
+      <c r="J68">
+        <v>1.93</v>
+      </c>
+      <c r="K68">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Intra-abdominal/hepatobiliary</t>
+        </is>
+      </c>
+      <c r="D69">
+        <v>16</v>
+      </c>
+      <c r="E69">
+        <v>925</v>
+      </c>
+      <c r="F69">
+        <v>4108</v>
+      </c>
+      <c r="G69">
+        <v>6344</v>
+      </c>
+      <c r="H69">
+        <v>34217</v>
+      </c>
+      <c r="I69">
+        <v>0.78</v>
+      </c>
+      <c r="J69">
+        <v>0.35</v>
+      </c>
+      <c r="K69">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Urinary tract</t>
+        </is>
+      </c>
+      <c r="D70">
+        <v>15</v>
+      </c>
+      <c r="E70">
+        <v>883</v>
+      </c>
+      <c r="F70">
+        <v>3978</v>
+      </c>
+      <c r="G70">
+        <v>13291</v>
+      </c>
+      <c r="H70">
+        <v>32645</v>
+      </c>
+      <c r="I70">
+        <v>0.67</v>
+      </c>
+      <c r="J70">
+        <v>0.26</v>
+      </c>
+      <c r="K70">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Mixed/unspecified</t>
+        </is>
+      </c>
+      <c r="D71">
+        <v>13</v>
+      </c>
+      <c r="E71">
+        <v>1018</v>
+      </c>
+      <c r="F71">
+        <v>3863</v>
+      </c>
+      <c r="G71">
+        <v>11019</v>
+      </c>
+      <c r="H71">
+        <v>57811</v>
+      </c>
+      <c r="I71">
+        <v>1.02</v>
+      </c>
+      <c r="J71">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="K71">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Catheter-related site</t>
+        </is>
+      </c>
+      <c r="D72">
+        <v>12</v>
+      </c>
+      <c r="E72">
+        <v>665</v>
+      </c>
+      <c r="F72">
+        <v>2503</v>
+      </c>
+      <c r="G72">
+        <v>541</v>
+      </c>
+      <c r="H72">
+        <v>4561</v>
+      </c>
+      <c r="I72">
+        <v>2.84</v>
+      </c>
+      <c r="J72">
+        <v>1.75</v>
+      </c>
+      <c r="K72">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Primary BSI</t>
+        </is>
+      </c>
+      <c r="D73">
+        <v>9</v>
+      </c>
+      <c r="E73">
+        <v>438</v>
+      </c>
+      <c r="F73">
+        <v>1660</v>
+      </c>
+      <c r="G73">
+        <v>1075</v>
+      </c>
+      <c r="H73">
+        <v>3212</v>
+      </c>
+      <c r="I73">
+        <v>0.46</v>
+      </c>
+      <c r="J73">
+        <v>0.15</v>
+      </c>
+      <c r="K73">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Skin/soft tissue</t>
+        </is>
+      </c>
+      <c r="D74">
+        <v>8</v>
+      </c>
+      <c r="E74">
+        <v>8777</v>
+      </c>
+      <c r="F74">
+        <v>45956</v>
+      </c>
+      <c r="G74">
+        <v>8103</v>
+      </c>
+      <c r="H74">
+        <v>50271</v>
+      </c>
+      <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74">
+        <v>1.61</v>
+      </c>
+      <c r="K74">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Bone/joint</t>
+        </is>
+      </c>
+      <c r="D75">
+        <v>7</v>
+      </c>
+      <c r="E75">
+        <v>8231</v>
+      </c>
+      <c r="F75">
+        <v>46056</v>
+      </c>
+      <c r="G75">
+        <v>10389</v>
+      </c>
+      <c r="H75">
+        <v>49320</v>
+      </c>
+      <c r="I75">
+        <v>1.72</v>
+      </c>
+      <c r="J75">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="K75">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Endocarditis</t>
+        </is>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76">
+        <v>4503</v>
+      </c>
+      <c r="F76">
+        <v>44970</v>
+      </c>
+      <c r="G76">
+        <v>6584</v>
+      </c>
+      <c r="H76">
+        <v>48038</v>
+      </c>
+      <c r="I76">
+        <v>0.7</v>
+      </c>
+      <c r="J76">
+        <v>0.58</v>
+      </c>
+      <c r="K76">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Mucosal barrier injury</t>
+        </is>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>42</v>
+      </c>
+      <c r="F77">
+        <v>77</v>
+      </c>
+      <c r="G77">
+        <v>52</v>
+      </c>
+      <c r="H77">
+        <v>167</v>
+      </c>
+      <c r="I77">
+        <v>2.65</v>
+      </c>
+      <c r="J77">
+        <v>2.65</v>
+      </c>
+      <c r="K77">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
           <t>Prior colonization or infection</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Prior colonization or infection</t>
-        </is>
-      </c>
-      <c r="D54">
-        <v>28</v>
-      </c>
-      <c r="E54">
-        <v>5880</v>
-      </c>
-      <c r="F54">
-        <v>38251</v>
-      </c>
-      <c r="G54">
-        <v>1276</v>
-      </c>
-      <c r="H54">
-        <v>3019</v>
-      </c>
-      <c r="I54">
-        <v>4.365</v>
-      </c>
-      <c r="J54">
-        <v>2.595</v>
-      </c>
-      <c r="K54">
-        <v>10.63</v>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Prior infection</t>
+        </is>
+      </c>
+      <c r="D78">
+        <v>23</v>
+      </c>
+      <c r="E78">
+        <v>1044</v>
+      </c>
+      <c r="F78">
+        <v>5110</v>
+      </c>
+      <c r="G78">
+        <v>2655</v>
+      </c>
+      <c r="H78">
+        <v>34587</v>
+      </c>
+      <c r="I78">
+        <v>4.06</v>
+      </c>
+      <c r="J78">
+        <v>3.2</v>
+      </c>
+      <c r="K78">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Prior colonization</t>
+        </is>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="E79">
+        <v>1030</v>
+      </c>
+      <c r="F79">
+        <v>3205</v>
+      </c>
+      <c r="G79">
+        <v>899</v>
+      </c>
+      <c r="H79">
+        <v>6632</v>
+      </c>
+      <c r="I79">
+        <v>6.18</v>
+      </c>
+      <c r="J79">
+        <v>4.05</v>
+      </c>
+      <c r="K79">
+        <v>16.12</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Prior colonization or infection (unspecified)</t>
+        </is>
+      </c>
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80">
+        <v>181</v>
+      </c>
+      <c r="F80">
+        <v>755</v>
+      </c>
+      <c r="G80">
+        <v>180</v>
+      </c>
+      <c r="H80">
+        <v>4462</v>
+      </c>
+      <c r="I80">
+        <v>7.6</v>
+      </c>
+      <c r="J80">
+        <v>4.1</v>
+      </c>
+      <c r="K80">
+        <v>27.05</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Prior immunosuppression treatment</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Prior immunosuppression, cancer treatment/corticosteroid use</t>
+        </is>
+      </c>
+      <c r="D81">
+        <v>15</v>
+      </c>
+      <c r="E81">
+        <v>519</v>
+      </c>
+      <c r="F81">
+        <v>1836</v>
+      </c>
+      <c r="G81">
+        <v>1488</v>
+      </c>
+      <c r="H81">
+        <v>6827</v>
+      </c>
+      <c r="I81">
+        <v>2.04</v>
+      </c>
+      <c r="J81">
+        <v>1.54</v>
+      </c>
+      <c r="K81">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Univariate and multivariate datasets created and categorized in L1 and L2 in a standardized way. Need to add L3, also what for references?
</commit_message>
<xml_diff>
--- a/categorical_summary.xlsx
+++ b/categorical_summary.xlsx
@@ -1,21 +1,360 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msfintl-my.sharepoint.com/personal/krystel_moussally_msf_org/Documents/OneDrive Updated/7_MENA branch/MEMU/WHO_EWI/AMR_ProxyInd/Analysis/R-project/scoping_amr_indicators/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_765FDFC08F79A8D366075C52F37BD272AA405214" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0709D624-43A6-4D7C-AF70-1AF4412AF771}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="5140" yWindow="1440" windowWidth="14400" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
+  <si>
+    <t>indicatorcategory_level1</t>
+  </si>
+  <si>
+    <t>indicatorcategory_level2</t>
+  </si>
+  <si>
+    <t>indicatorcategory_level3</t>
+  </si>
+  <si>
+    <t>n_studies</t>
+  </si>
+  <si>
+    <t>exposed_R</t>
+  </si>
+  <si>
+    <t>total_R</t>
+  </si>
+  <si>
+    <t>exposed_S</t>
+  </si>
+  <si>
+    <t>total_S</t>
+  </si>
+  <si>
+    <t>median_or</t>
+  </si>
+  <si>
+    <t>q25_or</t>
+  </si>
+  <si>
+    <t>q75_or</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hospital/care setting characteristics</t>
+  </si>
+  <si>
+    <t>Admission &amp; ward characteristics</t>
+  </si>
+  <si>
+    <t>Hospital-level characteristics</t>
+  </si>
+  <si>
+    <t>Antibiotic exposure</t>
+  </si>
+  <si>
+    <t>Prior antibiotic exposure, specific choice</t>
+  </si>
+  <si>
+    <t>Beta-lactams</t>
+  </si>
+  <si>
+    <t>Carbapenems</t>
+  </si>
+  <si>
+    <t>Cephems</t>
+  </si>
+  <si>
+    <t>Fluoroquinolones</t>
+  </si>
+  <si>
+    <t>Glycopeptides/oxazolidinones</t>
+  </si>
+  <si>
+    <t>Other classes</t>
+  </si>
+  <si>
+    <t>Tigecycline</t>
+  </si>
+  <si>
+    <t>Prior antibiotic exposure, non specific</t>
+  </si>
+  <si>
+    <t>In-hospital antibiotic exposure, non specific</t>
+  </si>
+  <si>
+    <t>In-hospital antibiotic exposure, specific</t>
+  </si>
+  <si>
+    <t>Biomedical results</t>
+  </si>
+  <si>
+    <t>Hematology markers</t>
+  </si>
+  <si>
+    <t>Liver markers</t>
+  </si>
+  <si>
+    <t>Metabolic markers</t>
+  </si>
+  <si>
+    <t>Clinical presentation</t>
+  </si>
+  <si>
+    <t>Clinical severity, infection site</t>
+  </si>
+  <si>
+    <t>Clinical severity score</t>
+  </si>
+  <si>
+    <t>Clinical presentation, other than infection site</t>
+  </si>
+  <si>
+    <t>Comorbidities</t>
+  </si>
+  <si>
+    <t>Cancer/hematologic malignancy</t>
+  </si>
+  <si>
+    <t>Immunosuppression/ immunocompromised state</t>
+  </si>
+  <si>
+    <t>Kidney/ renal disease</t>
+  </si>
+  <si>
+    <t>Cardiovascular &amp; cerebrovascular disease</t>
+  </si>
+  <si>
+    <t>Liver/ Gastrointestinal/ biliary disease</t>
+  </si>
+  <si>
+    <t>Metabolic/endocrine</t>
+  </si>
+  <si>
+    <t>Respiratory disease</t>
+  </si>
+  <si>
+    <t>Neurologic/ cognitive/ functional status</t>
+  </si>
+  <si>
+    <t>Other chronic condition</t>
+  </si>
+  <si>
+    <t>Autoimmune/ rheumatologic/ collective tissue disease</t>
+  </si>
+  <si>
+    <t>Comorbidity score</t>
+  </si>
+  <si>
+    <t>Urologic disease</t>
+  </si>
+  <si>
+    <t>Underweight/malnutrition</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Male sex</t>
+  </si>
+  <si>
+    <t>Older age (cutoffs &gt;/= 60 years)</t>
+  </si>
+  <si>
+    <t>Young age (cutoffs &lt;/= 5 years)</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Socio-economic status</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>Healthcare exposure</t>
+  </si>
+  <si>
+    <t>Hospital-acquired</t>
+  </si>
+  <si>
+    <t>Prior hospitalisation</t>
+  </si>
+  <si>
+    <t>Healthcare associated, other than hospital-acquired or non specified if hospital</t>
+  </si>
+  <si>
+    <t>Community-acquired</t>
+  </si>
+  <si>
+    <t>Prior ICU stay</t>
+  </si>
+  <si>
+    <t>Long-term care facility</t>
+  </si>
+  <si>
+    <t>Invasive procedures/devices</t>
+  </si>
+  <si>
+    <t>Central venous/intravascular access &amp; dialysis</t>
+  </si>
+  <si>
+    <t>Airway/respiratory procedures</t>
+  </si>
+  <si>
+    <t>Urinary catheters/urinary procedures</t>
+  </si>
+  <si>
+    <t>Surgery/invasive operation</t>
+  </si>
+  <si>
+    <t>Gastrointestinal/biliary tubes &amp; abdominal drains</t>
+  </si>
+  <si>
+    <t>Transplant</t>
+  </si>
+  <si>
+    <t>Invasive devices/procedures, unspecified</t>
+  </si>
+  <si>
+    <t>Blood transfusion</t>
+  </si>
+  <si>
+    <t>Internal device/implant</t>
+  </si>
+  <si>
+    <t>Neonatal risk</t>
+  </si>
+  <si>
+    <t>Birthweight</t>
+  </si>
+  <si>
+    <t>Gestational age</t>
+  </si>
+  <si>
+    <t>Feeding type</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Invasive devices, unspecified</t>
+  </si>
+  <si>
+    <t>Patient outcomes</t>
+  </si>
+  <si>
+    <t>Mortality</t>
+  </si>
+  <si>
+    <t>Current ICU stay</t>
+  </si>
+  <si>
+    <t>Complications</t>
+  </si>
+  <si>
+    <t>Current hospitalisation duration</t>
+  </si>
+  <si>
+    <t>Cure</t>
+  </si>
+  <si>
+    <t>Treatment failure</t>
+  </si>
+  <si>
+    <t>Persistent bacteremia</t>
+  </si>
+  <si>
+    <t>Readmission</t>
+  </si>
+  <si>
+    <t>Fever</t>
+  </si>
+  <si>
+    <t>Primary site of infection</t>
+  </si>
+  <si>
+    <t>Respiratory tract/pulmonary</t>
+  </si>
+  <si>
+    <t>Intra-abdominal/hepatobiliary</t>
+  </si>
+  <si>
+    <t>Urinary tract</t>
+  </si>
+  <si>
+    <t>Mixed/unspecified</t>
+  </si>
+  <si>
+    <t>Catheter-related site</t>
+  </si>
+  <si>
+    <t>Primary BSI</t>
+  </si>
+  <si>
+    <t>Skin/soft tissue</t>
+  </si>
+  <si>
+    <t>Bone/joint</t>
+  </si>
+  <si>
+    <t>Endocarditis</t>
+  </si>
+  <si>
+    <t>Mucosal barrier injury</t>
+  </si>
+  <si>
+    <t>Prior colonization or infection</t>
+  </si>
+  <si>
+    <t>Prior infection</t>
+  </si>
+  <si>
+    <t>Prior colonization</t>
+  </si>
+  <si>
+    <t>Prior colonization or infection (unspecified)</t>
+  </si>
+  <si>
+    <t>Prior immunosuppression treatment</t>
+  </si>
+  <si>
+    <t>Prior immunosuppression, cancer treatment/corticosteroid use</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +402,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +454,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +488,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +523,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,80 +699,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B81"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44.26953125" customWidth="1"/>
+    <col min="2" max="2" width="64.54296875" customWidth="1"/>
+    <col min="3" max="3" width="70.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>indicatorcategory_level1</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>indicatorcategory_level2</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>indicatorcategory_level3</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>n_studies</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>exposed_R</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>total_R</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>exposed_S</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>total_S</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>median_or</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>q25_or</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>q75_or</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Hospital/care setting characteristics</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Admission &amp; ward characteristics</t>
-        </is>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -447,14 +777,12 @@
         <v>0.37</v>
       </c>
       <c r="K2">
-        <v>2.05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Hospital-level characteristics</t>
-        </is>
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -481,21 +809,15 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Antibiotic exposure</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Beta-lactams</t>
-        </is>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -513,7 +835,7 @@
         <v>9312</v>
       </c>
       <c r="I4">
-        <v>4.15</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="J4">
         <v>2.41</v>
@@ -522,16 +844,12 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Carbapenems</t>
-        </is>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="D5">
         <v>41</v>
@@ -555,19 +873,15 @@
         <v>4.01</v>
       </c>
       <c r="K5">
-        <v>9.550000000000001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cephems</t>
-        </is>
+        <v>9.5500000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6">
         <v>35</v>
@@ -594,16 +908,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Fluoroquinolones</t>
-        </is>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
       <c r="D7">
         <v>33</v>
@@ -630,16 +940,12 @@
         <v>6.17</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Glycopeptides/oxazolidinones</t>
-        </is>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
       </c>
       <c r="D8">
         <v>22</v>
@@ -657,25 +963,21 @@
         <v>6860</v>
       </c>
       <c r="I8">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J8">
         <v>3.48</v>
       </c>
       <c r="K8">
-        <v>8.460000000000001</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Other classes</t>
-        </is>
+        <v>8.4600000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -702,16 +1004,12 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, specific choice</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Tigecycline</t>
-        </is>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -732,17 +1030,15 @@
         <v>7.46</v>
       </c>
       <c r="J10">
-        <v>4.35</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="K10">
         <v>10.38</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Prior antibiotic exposure, non specific</t>
-        </is>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>23</v>
       </c>
       <c r="D11">
         <v>92</v>
@@ -769,11 +1065,9 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>In-hospital antibiotic exposure, non specific</t>
-        </is>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>24</v>
       </c>
       <c r="D12">
         <v>26</v>
@@ -800,11 +1094,9 @@
         <v>2.94</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>In-hospital antibiotic exposure, specific</t>
-        </is>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>25</v>
       </c>
       <c r="D13">
         <v>20</v>
@@ -828,19 +1120,15 @@
         <v>2.33</v>
       </c>
       <c r="K13">
-        <v>10.21</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Biomedical results</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Hematology markers</t>
-        </is>
+        <v>10.210000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
       </c>
       <c r="D14">
         <v>24</v>
@@ -867,11 +1155,9 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Liver markers</t>
-        </is>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>28</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -895,14 +1181,12 @@
         <v>3.35</v>
       </c>
       <c r="K15">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Metabolic markers</t>
-        </is>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -929,16 +1213,12 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Clinical presentation</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Clinical severity, infection site</t>
-        </is>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
       </c>
       <c r="D17">
         <v>31</v>
@@ -965,11 +1245,9 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Clinical severity score</t>
-        </is>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>32</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -987,7 +1265,7 @@
         <v>3700</v>
       </c>
       <c r="I18">
-        <v>2.18</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="J18">
         <v>0.75</v>
@@ -996,11 +1274,9 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Clinical presentation, other than infection site</t>
-        </is>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>33</v>
       </c>
       <c r="D19">
         <v>8</v>
@@ -1021,22 +1297,18 @@
         <v>1.74</v>
       </c>
       <c r="J19">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K19">
         <v>3.24</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Comorbidities</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Cancer/hematologic malignancy</t>
-        </is>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
       </c>
       <c r="D20">
         <v>52</v>
@@ -1054,7 +1326,7 @@
         <v>75990</v>
       </c>
       <c r="I20">
-        <v>1.11</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J20">
         <v>0.41</v>
@@ -1063,11 +1335,9 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Immunosuppression/ immunocompromised state</t>
-        </is>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>36</v>
       </c>
       <c r="D21">
         <v>33</v>
@@ -1094,11 +1364,9 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="22">
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Kidney/ renal disease</t>
-        </is>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>37</v>
       </c>
       <c r="D22">
         <v>30</v>
@@ -1125,11 +1393,9 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Cardiovascular &amp; cerebrovascular disease</t>
-        </is>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>38</v>
       </c>
       <c r="D23">
         <v>27</v>
@@ -1156,11 +1422,9 @@
         <v>4.57</v>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Liver/ Gastrointestinal/ biliary disease</t>
-        </is>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>39</v>
       </c>
       <c r="D24">
         <v>25</v>
@@ -1187,11 +1451,9 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="25">
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Metabolic/endocrine</t>
-        </is>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>40</v>
       </c>
       <c r="D25">
         <v>24</v>
@@ -1218,11 +1480,9 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Respiratory disease</t>
-        </is>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>41</v>
       </c>
       <c r="D26">
         <v>20</v>
@@ -1249,11 +1509,9 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="27">
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Neurologic/ cognitive/ functional status</t>
-        </is>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>42</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -1280,11 +1538,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28">
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Other chronic condition</t>
-        </is>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>43</v>
       </c>
       <c r="D28">
         <v>9</v>
@@ -1305,17 +1561,15 @@
         <v>2.82</v>
       </c>
       <c r="J28">
-        <v>2.18</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="K28">
         <v>3.57</v>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Autoimmune/ rheumatologic/ collective tissue disease</t>
-        </is>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>44</v>
       </c>
       <c r="D29">
         <v>6</v>
@@ -1342,11 +1596,9 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="30">
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Comorbidity score</t>
-        </is>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>45</v>
       </c>
       <c r="D30">
         <v>6</v>
@@ -1373,11 +1625,9 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="31">
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Urologic disease</t>
-        </is>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>46</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -1404,11 +1654,9 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="32">
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Underweight/malnutrition</t>
-        </is>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>47</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1435,16 +1683,12 @@
         <v>2.67</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Demographics</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Male sex</t>
-        </is>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
       </c>
       <c r="D33">
         <v>36</v>
@@ -1471,11 +1715,9 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="34">
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Older age (cutoffs &gt;/= 60 years)</t>
-        </is>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>50</v>
       </c>
       <c r="D34">
         <v>10</v>
@@ -1502,11 +1744,9 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="35">
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Young age (cutoffs &lt;/= 5 years)</t>
-        </is>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>51</v>
       </c>
       <c r="D35">
         <v>7</v>
@@ -1533,11 +1773,9 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="36">
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Ethnicity</t>
-        </is>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>52</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -1564,11 +1802,9 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="37">
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Socio-economic status</t>
-        </is>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>53</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -1595,11 +1831,9 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="38">
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Geography</t>
-        </is>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>54</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -1626,16 +1860,12 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Healthcare exposure</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Hospital-acquired</t>
-        </is>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
       </c>
       <c r="D39">
         <v>64</v>
@@ -1662,11 +1892,9 @@
         <v>5.88</v>
       </c>
     </row>
-    <row r="40">
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Prior hospitalisation</t>
-        </is>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>57</v>
       </c>
       <c r="D40">
         <v>48</v>
@@ -1693,11 +1921,9 @@
         <v>4.04</v>
       </c>
     </row>
-    <row r="41">
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Healthcare associated, other than hospital-acquired or non specified if hospital</t>
-        </is>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>58</v>
       </c>
       <c r="D41">
         <v>27</v>
@@ -1724,11 +1950,9 @@
         <v>6.58</v>
       </c>
     </row>
-    <row r="42">
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Community-acquired</t>
-        </is>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>59</v>
       </c>
       <c r="D42">
         <v>26</v>
@@ -1755,11 +1979,9 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Prior ICU stay</t>
-        </is>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>60</v>
       </c>
       <c r="D43">
         <v>24</v>
@@ -1777,7 +1999,7 @@
         <v>6621</v>
       </c>
       <c r="I43">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J43">
         <v>3.17</v>
@@ -1786,11 +2008,9 @@
         <v>7.33</v>
       </c>
     </row>
-    <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Long-term care facility</t>
-        </is>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>61</v>
       </c>
       <c r="D44">
         <v>16</v>
@@ -1817,16 +2037,12 @@
         <v>5.99</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Invasive procedures/devices</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Central venous/intravascular access &amp; dialysis</t>
-        </is>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
       </c>
       <c r="D45">
         <v>69</v>
@@ -1853,11 +2069,9 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="46">
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Airway/respiratory procedures</t>
-        </is>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>64</v>
       </c>
       <c r="D46">
         <v>59</v>
@@ -1875,20 +2089,18 @@
         <v>33227</v>
       </c>
       <c r="I46">
-        <v>4.36</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="J46">
-        <v>2.51</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="K46">
-        <v>8.199999999999999</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Urinary catheters/urinary procedures</t>
-        </is>
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>65</v>
       </c>
       <c r="D47">
         <v>50</v>
@@ -1909,17 +2121,15 @@
         <v>3.63</v>
       </c>
       <c r="J47">
-        <v>2.47</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="K47">
         <v>6.02</v>
       </c>
     </row>
-    <row r="48">
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Surgery/invasive operation</t>
-        </is>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>66</v>
       </c>
       <c r="D48">
         <v>46</v>
@@ -1946,11 +2156,9 @@
         <v>5.52</v>
       </c>
     </row>
-    <row r="49">
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Gastrointestinal/biliary tubes &amp; abdominal drains</t>
-        </is>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>67</v>
       </c>
       <c r="D49">
         <v>41</v>
@@ -1977,11 +2185,9 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="50">
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Transplant</t>
-        </is>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>68</v>
       </c>
       <c r="D50">
         <v>25</v>
@@ -2008,11 +2214,9 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="51">
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Invasive devices/procedures, unspecified</t>
-        </is>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>69</v>
       </c>
       <c r="D51">
         <v>13</v>
@@ -2039,11 +2243,9 @@
         <v>4.96</v>
       </c>
     </row>
-    <row r="52">
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Blood transfusion</t>
-        </is>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>70</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -2070,11 +2272,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53">
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Internal device/implant</t>
-        </is>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>71</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -2101,16 +2301,12 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Neonatal risk</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Birthweight</t>
-        </is>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" t="s">
+        <v>73</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -2137,11 +2333,9 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="55">
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Gestational age</t>
-        </is>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>74</v>
       </c>
       <c r="D55">
         <v>4</v>
@@ -2168,11 +2362,9 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="56">
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Feeding type</t>
-        </is>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>75</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2193,22 +2385,18 @@
         <v>1.83</v>
       </c>
       <c r="J56">
-        <v>1.13</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="K56">
-        <v>2.53</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" t="s">
+        <v>76</v>
       </c>
       <c r="D57">
         <v>47</v>
@@ -2235,11 +2423,9 @@
         <v>5.69</v>
       </c>
     </row>
-    <row r="58">
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Invasive devices, unspecified</t>
-        </is>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>77</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -2266,16 +2452,12 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Patient outcomes</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Mortality</t>
-        </is>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
       </c>
       <c r="D59">
         <v>90</v>
@@ -2302,11 +2484,9 @@
         <v>6.62</v>
       </c>
     </row>
-    <row r="60">
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Current ICU stay</t>
-        </is>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>80</v>
       </c>
       <c r="D60">
         <v>41</v>
@@ -2333,11 +2513,9 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="61">
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Complications</t>
-        </is>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>81</v>
       </c>
       <c r="D61">
         <v>13</v>
@@ -2355,7 +2533,7 @@
         <v>3811</v>
       </c>
       <c r="I61">
-        <v>2.51</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="J61">
         <v>2.12</v>
@@ -2364,11 +2542,9 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="62">
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Current hospitalisation duration</t>
-        </is>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>82</v>
       </c>
       <c r="D62">
         <v>9</v>
@@ -2395,11 +2571,9 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="63">
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Cure</t>
-        </is>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>83</v>
       </c>
       <c r="D63">
         <v>8</v>
@@ -2426,11 +2600,9 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="64">
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Treatment failure</t>
-        </is>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>84</v>
       </c>
       <c r="D64">
         <v>8</v>
@@ -2448,7 +2620,7 @@
         <v>2916</v>
       </c>
       <c r="I64">
-        <v>4.36</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="J64">
         <v>2.69</v>
@@ -2457,11 +2629,9 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="65">
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Persistent bacteremia</t>
-        </is>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>85</v>
       </c>
       <c r="D65">
         <v>6</v>
@@ -2488,11 +2658,9 @@
         <v>10.41</v>
       </c>
     </row>
-    <row r="66">
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Readmission</t>
-        </is>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>86</v>
       </c>
       <c r="D66">
         <v>4</v>
@@ -2519,11 +2687,9 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="67">
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Fever</t>
-        </is>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>87</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2550,16 +2716,12 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Primary site of infection</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Respiratory tract/pulmonary</t>
-        </is>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
       </c>
       <c r="D68">
         <v>26</v>
@@ -2586,11 +2748,9 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="69">
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Intra-abdominal/hepatobiliary</t>
-        </is>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>90</v>
       </c>
       <c r="D69">
         <v>16</v>
@@ -2617,11 +2777,9 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="70">
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Urinary tract</t>
-        </is>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>91</v>
       </c>
       <c r="D70">
         <v>15</v>
@@ -2648,11 +2806,9 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="71">
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Mixed/unspecified</t>
-        </is>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>92</v>
       </c>
       <c r="D71">
         <v>13</v>
@@ -2673,17 +2829,15 @@
         <v>1.02</v>
       </c>
       <c r="J71">
-        <v>0.5600000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K71">
         <v>2.44</v>
       </c>
     </row>
-    <row r="72">
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Catheter-related site</t>
-        </is>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>93</v>
       </c>
       <c r="D72">
         <v>12</v>
@@ -2710,11 +2864,9 @@
         <v>4.47</v>
       </c>
     </row>
-    <row r="73">
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Primary BSI</t>
-        </is>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>94</v>
       </c>
       <c r="D73">
         <v>9</v>
@@ -2741,11 +2893,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Skin/soft tissue</t>
-        </is>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>95</v>
       </c>
       <c r="D74">
         <v>8</v>
@@ -2772,11 +2922,9 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="75">
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Bone/joint</t>
-        </is>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>96</v>
       </c>
       <c r="D75">
         <v>7</v>
@@ -2797,17 +2945,15 @@
         <v>1.72</v>
       </c>
       <c r="J75">
-        <v>0.8100000000000001</v>
+        <v>0.81</v>
       </c>
       <c r="K75">
         <v>2.84</v>
       </c>
     </row>
-    <row r="76">
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Endocarditis</t>
-        </is>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>97</v>
       </c>
       <c r="D76">
         <v>3</v>
@@ -2828,17 +2974,15 @@
         <v>0.7</v>
       </c>
       <c r="J76">
-        <v>0.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K76">
         <v>1.79</v>
       </c>
     </row>
-    <row r="77">
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Mucosal barrier injury</t>
-        </is>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>98</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2865,16 +3009,12 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Prior colonization or infection</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Prior infection</t>
-        </is>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>99</v>
+      </c>
+      <c r="B78" t="s">
+        <v>100</v>
       </c>
       <c r="D78">
         <v>23</v>
@@ -2892,7 +3032,7 @@
         <v>34587</v>
       </c>
       <c r="I78">
-        <v>4.06</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="J78">
         <v>3.2</v>
@@ -2901,11 +3041,9 @@
         <v>8.24</v>
       </c>
     </row>
-    <row r="79">
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Prior colonization</t>
-        </is>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>101</v>
       </c>
       <c r="D79">
         <v>20</v>
@@ -2932,11 +3070,9 @@
         <v>16.12</v>
       </c>
     </row>
-    <row r="80">
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Prior colonization or infection (unspecified)</t>
-        </is>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>102</v>
       </c>
       <c r="D80">
         <v>5</v>
@@ -2957,22 +3093,18 @@
         <v>7.6</v>
       </c>
       <c r="J80">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K80">
         <v>27.05</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Prior immunosuppression treatment</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Prior immunosuppression, cancer treatment/corticosteroid use</t>
-        </is>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" t="s">
+        <v>104</v>
       </c>
       <c r="D81">
         <v>15</v>

</xml_diff>